<commit_message>
Add NextCheckInMinutes to Event and fine-tune reporting logic
The mandatory NextCheckInMinutes property has been added to the Event entity and its configuration in EF Core, including database migration. Event creation in MonitorJob has been updated to use the monitor interval. The downTime calculation in ReportService now adds NextCheckInMinutes from events, improving accuracy and simplicity. Tests have been updated and NextCheckInMinutes and IsImportant are encapsulated as read-only.
</commit_message>
<xml_diff>
--- a/Uptime.Stars.Backend/Uptime.Stars.Api/Resources/ReportTemplate.xlsx
+++ b/Uptime.Stars.Backend/Uptime.Stars.Api/Resources/ReportTemplate.xlsx
@@ -1,13 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseb\source\repos\Hackaton\uptime-stars-backend\Uptime.Stars.Backend\Uptime.Stars.Api\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19959433-410F-4525-BE96-6B7015B204CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="SLA General" sheetId="1" r:id="rId4"/>
+    <sheet name="SLA General" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="2Emx+jdxbLZ//7ufQ7CEu+FrG4keM1qGOQ18w0fVZKs="/>
     </ext>
@@ -44,18 +64,18 @@
   <si>
     <r>
       <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
-        <b/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
       </rPr>
       <t>Data de 1 mes</t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
       </rPr>
       <t xml:space="preserve"> (horas)</t>
     </r>
@@ -136,62 +156,65 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="22.0"/>
+      <sz val="22"/>
       <color theme="0"/>
       <name val="Amasis MT Pro Black"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+    </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="0"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="ADLaM Display"/>
     </font>
@@ -201,7 +224,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -277,49 +300,89 @@
     </fill>
   </fills>
   <borders count="75">
-    <border/>
-    <border>
-      <left/>
-      <top/>
-    </border>
-    <border>
-      <top/>
-    </border>
-    <border>
-      <right/>
-      <top/>
-    </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
       <bottom/>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom/>
-    </border>
-    <border>
-      <right/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
-    </border>
-    <border>
-      <right/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -332,6 +395,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -346,19 +410,23 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -368,27 +436,34 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color theme="0"/>
       </left>
+      <right/>
       <top style="thin">
         <color theme="0"/>
       </top>
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="0"/>
       </top>
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color theme="0"/>
       </right>
@@ -398,14 +473,18 @@
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -413,208 +492,23 @@
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <bottom/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="0"/>
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -626,92 +520,352 @@
       <top style="thin">
         <color theme="0"/>
       </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
-    </border>
-    <border>
-      <left/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
       <top/>
       <bottom/>
-    </border>
-    <border>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color theme="0"/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-    </border>
-    <border>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
       <right style="thin">
         <color theme="0"/>
       </right>
       <top style="thin">
         <color theme="0"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color theme="0"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color theme="0"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color theme="0"/>
       </left>
+      <right/>
       <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color theme="0"/>
       </bottom>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color theme="0"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -724,19 +878,23 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -746,15 +904,18 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
         <color theme="0"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -769,19 +930,23 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -791,6 +956,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -802,6 +968,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -816,19 +984,23 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -838,8 +1010,10 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="medium">
         <color rgb="FF000000"/>
@@ -847,19 +1021,27 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color theme="0"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -872,280 +1054,306 @@
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color theme="0"/>
       </left>
+      <right/>
       <top style="thin">
         <color theme="0"/>
       </top>
       <bottom/>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color theme="0"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color theme="0"/>
       </left>
-    </border>
-    <border>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="0"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
+      <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+  <cellXfs count="113">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="8" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="13" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="12" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="5" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="8" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="8" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="8" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="8" fillId="7" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="5" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="5" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="14" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="20" fillId="0" fontId="6" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="7" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="21" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="6" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="22" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="23" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="6" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="24" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="0" fontId="6" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="26" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="27" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="28" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="29" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="30" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="31" fillId="8" fontId="10" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="32" fillId="7" fontId="7" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="46" fontId="7" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="7" fillId="7" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="33" fillId="7" fontId="7" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="13" fillId="9" fontId="5" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="26" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="34" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="35" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="36" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="37" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="38" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="39" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="40" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="7" fontId="8" numFmtId="46" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="41" fillId="7" fontId="8" numFmtId="46" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="42" fillId="7" fontId="8" numFmtId="46" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="43" fillId="7" fontId="8" numFmtId="46" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="44" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="45" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="46" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="47" fillId="7" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="7" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="48" fillId="7" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="41" fillId="7" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="49" fillId="7" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="42" fillId="7" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="10" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="50" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="14" fillId="11" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="47" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="14" fillId="10" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="14" fillId="11" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="51" fillId="7" fontId="7" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="52" fillId="12" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="53" fillId="12" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="54" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="55" fillId="13" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="56" fillId="13" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="57" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="58" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="59" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="60" fillId="0" fontId="6" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="61" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="59" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="46" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="62" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="63" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="64" fillId="0" fontId="6" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="65" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="12" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="66" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="12" fontId="5" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="14" fillId="13" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="13" fillId="13" fontId="5" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="52" fillId="12" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="52" fillId="13" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="53" fillId="13" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="67" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="68" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="48" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="16" fillId="7" fontId="7" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="4" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="69" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="70" fillId="7" fontId="7" numFmtId="46" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="71" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="72" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="73" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="10" fontId="9" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="13" fillId="11" fontId="9" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="74" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1162,7 +1370,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" i="0">
+              <a:rPr lang="es-PE" b="0" i="0">
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
@@ -1175,10 +1383,13 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1192,20 +1403,28 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="1"/>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr lvl="0">
-                  <a:defRPr b="1" i="0" sz="1000">
+                  <a:defRPr sz="1000" b="1" i="0">
                     <a:solidFill>
                       <a:srgbClr val="FFFFFF"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -1214,19 +1433,83 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'SLA General'!$N$17:$Q$17</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Depósitos %</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Retiros %</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Validaciones %</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Validaciones %</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'SLA General'!$N$18:$Q$18</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                  <a:ln cmpd="sng">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6286-41E1-B0B4-8E83F9F2D505}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="940351104"/>
         <c:axId val="290878251"/>
       </c:barChart>
@@ -1251,15 +1534,7 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1268,22 +1543,28 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0" i="0" sz="900">
+              <a:defRPr sz="900" b="0" i="0">
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="290878251"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="290878251"/>
@@ -1306,21 +1587,13 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1339,23 +1612,37 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="940351104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:schemeClr val="lt1"/>
     </a:solidFill>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1364,7 +1651,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0" i="0" sz="1400">
+              <a:defRPr sz="1400" b="0" i="0">
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
@@ -1372,7 +1659,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" i="0" sz="1400">
+              <a:rPr lang="es-PE" sz="1400" b="0" i="0">
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
@@ -1385,10 +1672,13 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1402,20 +1692,28 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="1"/>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr lvl="0">
-                  <a:defRPr b="1" i="0" sz="1000">
+                  <a:defRPr sz="1000" b="1" i="0">
                     <a:solidFill>
                       <a:srgbClr val="FFFFFF"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -1424,19 +1722,83 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'SLA General'!$N$10:$Q$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Depósitos %</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Retiros %</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Validaciones %</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Validaciones %</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'SLA General'!$N$11:$Q$11</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                  <a:ln cmpd="sng">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4986-4FF9-BDF3-DDCF6BCEE16D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="1140615774"/>
         <c:axId val="1441410886"/>
       </c:barChart>
@@ -1461,15 +1823,7 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1478,22 +1832,28 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0" i="0" sz="900">
+              <a:defRPr sz="900" b="0" i="0">
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1441410886"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="1441410886"/>
@@ -1516,21 +1876,13 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1549,23 +1901,33 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1140615774"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:schemeClr val="lt1"/>
     </a:solidFill>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
@@ -1574,9 +1936,15 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5505450" cy="2428875"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="710771122" name="Chart 1"/>
+        <xdr:cNvPr id="710771122" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000B2815D2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1585,7 +1953,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1599,9 +1967,15 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5514975" cy="2609850"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1870833995" name="Chart 2"/>
+        <xdr:cNvPr id="1870833995" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004BA9826F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1610,7 +1984,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1624,9 +1998,15 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="485775" cy="323850"/>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Shape 3"/>
+        <xdr:cNvPr id="3" name="Shape 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1636,8 +2016,8 @@
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
-            <a:gd fmla="val 50000" name="adj1"/>
-            <a:gd fmla="val 50000" name="adj2"/>
+            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj2" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -1648,12 +2028,12 @@
         </a:ln>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr anchorCtr="0" anchor="t" bIns="45700" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="45700">
+        <a:bodyPr spcFirstLastPara="1" wrap="square" lIns="91425" tIns="45700" rIns="91425" bIns="45700" anchor="t" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" rtl="0">
             <a:spcBef>
               <a:spcPts val="0"/>
             </a:spcBef>
@@ -1662,9 +2042,6 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:r>
-            <a:t/>
-          </a:r>
           <a:endParaRPr sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -1675,7 +2052,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1865,680 +2242,686 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:S1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:D29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.38"/>
-    <col customWidth="1" min="2" max="2" width="26.5"/>
-    <col customWidth="1" min="3" max="3" width="9.5"/>
-    <col customWidth="1" min="4" max="5" width="8.0"/>
-    <col customWidth="1" min="6" max="6" width="13.88"/>
-    <col customWidth="1" min="7" max="7" width="21.88"/>
-    <col customWidth="1" min="8" max="8" width="13.0"/>
-    <col customWidth="1" min="9" max="9" width="10.5"/>
-    <col customWidth="1" min="10" max="10" width="4.13"/>
-    <col customWidth="1" min="11" max="11" width="0.88"/>
-    <col customWidth="1" min="12" max="12" width="0.63"/>
-    <col customWidth="1" min="13" max="13" width="3.5"/>
-    <col customWidth="1" min="14" max="14" width="13.63"/>
-    <col customWidth="1" min="15" max="15" width="13.0"/>
-    <col customWidth="1" min="16" max="16" width="14.13"/>
-    <col customWidth="1" min="17" max="17" width="14.38"/>
-    <col customWidth="1" min="18" max="26" width="8.88"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="10" max="10" width="4.109375" customWidth="1"/>
+    <col min="11" max="11" width="0.88671875" customWidth="1"/>
+    <col min="12" max="12" width="0.6640625" customWidth="1"/>
+    <col min="13" max="13" width="3.44140625" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="14.109375" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" customWidth="1"/>
+    <col min="18" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="15.0" customHeight="1">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:19" ht="15" customHeight="1">
+      <c r="B2" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
     </row>
-    <row r="3" ht="15.0" customHeight="1">
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
+    <row r="3" spans="2:19" ht="15" customHeight="1">
+      <c r="B3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
     </row>
-    <row r="4" ht="7.5" customHeight="1"/>
-    <row r="5">
-      <c r="B5" s="9" t="s">
+    <row r="4" spans="2:19" ht="7.5" customHeight="1"/>
+    <row r="5" spans="2:19" ht="18">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="K5" s="10"/>
-      <c r="N5" s="11" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="K5" s="101"/>
+      <c r="N5" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="3"/>
+      <c r="O5" s="96"/>
+      <c r="P5" s="96"/>
+      <c r="Q5" s="96"/>
+      <c r="R5" s="96"/>
+      <c r="S5" s="97"/>
     </row>
-    <row r="6">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="2:19" ht="18">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="K6" s="12"/>
-      <c r="N6" s="13"/>
-      <c r="S6" s="14"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="K6" s="102"/>
+      <c r="N6" s="105"/>
+      <c r="O6" s="106"/>
+      <c r="P6" s="106"/>
+      <c r="Q6" s="106"/>
+      <c r="R6" s="106"/>
+      <c r="S6" s="107"/>
     </row>
-    <row r="7">
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="2:19" ht="18">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="K7" s="12"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="8"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="K7" s="102"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="99"/>
+      <c r="P7" s="99"/>
+      <c r="Q7" s="99"/>
+      <c r="R7" s="99"/>
+      <c r="S7" s="100"/>
     </row>
-    <row r="8">
-      <c r="K8" s="12"/>
+    <row r="8" spans="2:19" ht="14.4">
+      <c r="K8" s="102"/>
     </row>
-    <row r="9">
-      <c r="B9" s="15" t="s">
+    <row r="9" spans="2:19" ht="14.4">
+      <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="18">
-        <v>720.0</v>
-      </c>
-      <c r="H9" s="19" t="s">
+      <c r="G9" s="7">
+        <v>720</v>
+      </c>
+      <c r="H9" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="K9" s="12"/>
-      <c r="N9" s="21" t="s">
+      <c r="I9" s="70"/>
+      <c r="K9" s="102"/>
+      <c r="N9" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="23"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
-    <row r="10">
-      <c r="B10" s="24" t="s">
+    <row r="10" spans="2:19" ht="14.4">
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="9">
         <f>SUM(D33,I33)</f>
-        <v>0.1041666667</v>
-      </c>
-      <c r="K10" s="12"/>
-      <c r="N10" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="102"/>
+      <c r="N10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O10" s="26" t="s">
+      <c r="O10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P10" s="27" t="s">
+      <c r="P10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="Q10" s="28" t="s">
+      <c r="Q10" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" s="29" t="s">
+    <row r="11" spans="2:19" ht="14.4">
+      <c r="B11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="14">
         <f>SUM(D24,I24)</f>
-        <v>1.3125</v>
-      </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="82"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="36">
+      <c r="G11" s="60"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="53">
         <f>((G9-C12)-(C10+C11))/G9*100</f>
-        <v>99.60648148</v>
-      </c>
-      <c r="K11" s="12"/>
-      <c r="N11" s="37">
+        <v>100</v>
+      </c>
+      <c r="K11" s="102"/>
+      <c r="N11" s="55">
         <f>((G9-N13)-(C29+C20))/G9*100</f>
-        <v>99.97106481</v>
-      </c>
-      <c r="O11" s="38">
+        <v>100</v>
+      </c>
+      <c r="O11" s="57">
         <f>((G9-O13)-(C30+C21))/G9*100</f>
         <v>100</v>
       </c>
-      <c r="P11" s="37">
+      <c r="P11" s="55">
         <f>((G9-P13)-(C31+C22))/G9*100</f>
         <v>100</v>
       </c>
-      <c r="Q11" s="37">
+      <c r="Q11" s="55">
         <f>((G9-Q13)-(C32+C23))/G9*100</f>
         <v>100</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="39" t="s">
+    <row r="12" spans="2:19" ht="14.4">
+      <c r="B12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="16">
         <f>SUM(C10:C11)</f>
-        <v>1.416666667</v>
-      </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="45"/>
-      <c r="K12" s="12"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="48"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="84"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="54"/>
+      <c r="K12" s="102"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="109"/>
     </row>
-    <row r="13">
-      <c r="K13" s="12"/>
-      <c r="N13" s="49">
+    <row r="13" spans="2:19" ht="14.4">
+      <c r="K13" s="102"/>
+      <c r="N13" s="17">
         <f>SUM(C20,C29)</f>
-        <v>0.1041666667</v>
-      </c>
-      <c r="O13" s="50">
+        <v>0</v>
+      </c>
+      <c r="O13" s="18">
         <f>SUM(C21,C30)</f>
         <v>0</v>
       </c>
-      <c r="P13" s="51">
+      <c r="P13" s="19">
         <f>SUM(C22,C31)</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="52">
+      <c r="Q13" s="20">
         <f>SUM(C23,C32)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" ht="4.5" customHeight="1">
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="55"/>
-      <c r="K14" s="12"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="58"/>
+    <row r="14" spans="2:19" ht="4.5" customHeight="1">
+      <c r="B14" s="65"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="67"/>
+      <c r="K14" s="102"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="23"/>
     </row>
-    <row r="15">
-      <c r="K15" s="12"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="60"/>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="61"/>
+    <row r="15" spans="2:19" ht="14.4">
+      <c r="K15" s="102"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="26"/>
     </row>
-    <row r="16">
-      <c r="B16" s="62" t="s">
+    <row r="16" spans="2:19" ht="14.4">
+      <c r="B16" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="64"/>
-      <c r="G16" s="65" t="s">
+      <c r="C16" s="69"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="27"/>
+      <c r="G16" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="63"/>
-      <c r="I16" s="20"/>
-      <c r="K16" s="12"/>
-      <c r="N16" s="21" t="s">
+      <c r="H16" s="69"/>
+      <c r="I16" s="70"/>
+      <c r="K16" s="102"/>
+      <c r="N16" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="23"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="73"/>
+      <c r="Q16" s="74"/>
     </row>
-    <row r="17">
-      <c r="B17" s="66"/>
-      <c r="K17" s="12"/>
-      <c r="N17" s="67" t="s">
+    <row r="17" spans="2:17" ht="14.4">
+      <c r="B17" s="28"/>
+      <c r="K17" s="102"/>
+      <c r="N17" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="O17" s="27" t="s">
+      <c r="O17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="P17" s="27" t="s">
+      <c r="P17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="Q17" s="27" t="s">
+      <c r="Q17" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18">
-      <c r="B18" s="68" t="s">
+    <row r="18" spans="2:17" ht="14.4">
+      <c r="B18" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="63"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="69"/>
-      <c r="G18" s="70" t="s">
+      <c r="C18" s="69"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="30"/>
+      <c r="G18" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="63"/>
-      <c r="I18" s="20"/>
-      <c r="K18" s="12"/>
-      <c r="N18" s="38">
+      <c r="H18" s="69"/>
+      <c r="I18" s="70"/>
+      <c r="K18" s="102"/>
+      <c r="N18" s="57">
         <f>((G9-N20)-(H29+H20))/G9*100</f>
-        <v>99.65277778</v>
-      </c>
-      <c r="O18" s="37">
+        <v>100</v>
+      </c>
+      <c r="O18" s="55">
         <f>((G9-O20)-(H30+H21))/G9*100</f>
-        <v>99.98263889</v>
-      </c>
-      <c r="P18" s="37">
+        <v>100</v>
+      </c>
+      <c r="P18" s="55">
         <f>((G9-P20)-(H31+H22))/G9*100</f>
         <v>100</v>
       </c>
-      <c r="Q18" s="71">
+      <c r="Q18" s="75">
         <f>((G9-Q20)-(H32+H23))/G9*100</f>
         <v>100</v>
       </c>
     </row>
-    <row r="19">
-      <c r="B19" s="72" t="s">
+    <row r="19" spans="2:17" ht="14.4">
+      <c r="B19" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="74"/>
-      <c r="E19" s="64"/>
-      <c r="G19" s="75" t="s">
+      <c r="D19" s="111"/>
+      <c r="E19" s="27"/>
+      <c r="G19" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="76" t="s">
+      <c r="H19" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="77"/>
-      <c r="K19" s="12"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
-      <c r="Q19" s="78"/>
+      <c r="I19" s="79"/>
+      <c r="K19" s="102"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="56"/>
+      <c r="P19" s="56"/>
+      <c r="Q19" s="76"/>
     </row>
-    <row r="20">
-      <c r="B20" s="79" t="s">
+    <row r="20" spans="2:17" ht="14.4">
+      <c r="B20" s="33" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="80">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D20" s="81"/>
-      <c r="E20" s="82"/>
-      <c r="G20" s="83" t="s">
+      <c r="E20" s="34"/>
+      <c r="G20" s="35" t="s">
         <v>23</v>
       </c>
       <c r="H20" s="80">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="I20" s="81"/>
-      <c r="K20" s="12"/>
-      <c r="N20" s="84">
+      <c r="K20" s="102"/>
+      <c r="N20" s="36">
         <f>SUM(H20,H29)</f>
-        <v>1.25</v>
-      </c>
-      <c r="O20" s="84">
+        <v>0</v>
+      </c>
+      <c r="O20" s="36">
         <f>SUM(H21,H30)</f>
-        <v>0.0625</v>
-      </c>
-      <c r="P20" s="84">
+        <v>0</v>
+      </c>
+      <c r="P20" s="36">
         <f>SUM(H22,H31)</f>
         <v>0</v>
       </c>
-      <c r="Q20" s="84">
+      <c r="Q20" s="36">
         <f>SUM(H23,H32)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="79" t="s">
+    <row r="21" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B21" s="33" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="80">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D21" s="81"/>
-      <c r="E21" s="82"/>
-      <c r="G21" s="83" t="s">
+      <c r="E21" s="34"/>
+      <c r="G21" s="35" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="80">
-        <v>0.0625</v>
+        <v>0</v>
       </c>
       <c r="I21" s="81"/>
-      <c r="K21" s="12"/>
+      <c r="K21" s="102"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="79" t="s">
+    <row r="22" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B22" s="33" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="80">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D22" s="81"/>
-      <c r="E22" s="82"/>
-      <c r="G22" s="83" t="s">
+      <c r="E22" s="34"/>
+      <c r="G22" s="35" t="s">
         <v>26</v>
       </c>
       <c r="H22" s="80">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I22" s="81"/>
-      <c r="K22" s="12"/>
+      <c r="K22" s="102"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="85" t="s">
+    <row r="23" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B23" s="37" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="80">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D23" s="81"/>
-      <c r="E23" s="82"/>
-      <c r="G23" s="86" t="s">
+      <c r="E23" s="34"/>
+      <c r="G23" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="87">
-        <v>0.0</v>
-      </c>
-      <c r="I23" s="88"/>
-      <c r="K23" s="12"/>
+      <c r="H23" s="86">
+        <v>0</v>
+      </c>
+      <c r="I23" s="87"/>
+      <c r="K23" s="102"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="89" t="s">
+    <row r="24" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B24" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="90"/>
-      <c r="D24" s="91">
+      <c r="C24" s="89"/>
+      <c r="D24" s="39">
         <f>SUM(C20:D23)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="66"/>
-      <c r="G24" s="92" t="s">
+      <c r="E24" s="28"/>
+      <c r="G24" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="90"/>
-      <c r="I24" s="93">
+      <c r="H24" s="89"/>
+      <c r="I24" s="40">
         <f>SUM(H20:I23)</f>
-        <v>1.3125</v>
-      </c>
-      <c r="K24" s="12"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="102"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="K25" s="12"/>
+    <row r="25" spans="2:17" ht="15.75" customHeight="1">
+      <c r="K25" s="102"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="K26" s="12"/>
+    <row r="26" spans="2:17" ht="15.75" customHeight="1">
+      <c r="K26" s="102"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="68" t="s">
+    <row r="27" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B27" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="63"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="69"/>
-      <c r="G27" s="70" t="s">
+      <c r="C27" s="69"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="30"/>
+      <c r="G27" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="H27" s="63"/>
-      <c r="I27" s="20"/>
-      <c r="K27" s="12"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="70"/>
+      <c r="K27" s="102"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="94" t="s">
+    <row r="28" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B28" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="73" t="s">
+      <c r="C28" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="74"/>
-      <c r="E28" s="64"/>
-      <c r="G28" s="95" t="s">
+      <c r="D28" s="111"/>
+      <c r="E28" s="27"/>
+      <c r="G28" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="96" t="s">
+      <c r="H28" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="I28" s="74"/>
-      <c r="K28" s="12"/>
+      <c r="I28" s="111"/>
+      <c r="K28" s="102"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="83" t="s">
+    <row r="29" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B29" s="35" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="80">
-        <v>0.10416666666666667</v>
+        <v>0</v>
       </c>
       <c r="D29" s="81"/>
-      <c r="E29" s="82"/>
-      <c r="G29" s="83" t="s">
+      <c r="E29" s="34"/>
+      <c r="G29" s="35" t="s">
         <v>23</v>
       </c>
       <c r="H29" s="80">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I29" s="81"/>
-      <c r="K29" s="12"/>
+      <c r="K29" s="102"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="83" t="s">
+    <row r="30" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B30" s="35" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="80">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D30" s="81"/>
-      <c r="E30" s="82"/>
-      <c r="G30" s="83" t="s">
+      <c r="E30" s="34"/>
+      <c r="G30" s="35" t="s">
         <v>24</v>
       </c>
       <c r="H30" s="80">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I30" s="81"/>
-      <c r="K30" s="12"/>
+      <c r="K30" s="102"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="83" t="s">
+    <row r="31" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B31" s="35" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="80">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D31" s="81"/>
-      <c r="E31" s="82"/>
-      <c r="G31" s="83" t="s">
+      <c r="E31" s="34"/>
+      <c r="G31" s="35" t="s">
         <v>25</v>
       </c>
       <c r="H31" s="80">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I31" s="81"/>
-      <c r="K31" s="12"/>
+      <c r="K31" s="102"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="86" t="s">
+    <row r="32" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B32" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="87">
-        <v>0.0</v>
-      </c>
-      <c r="D32" s="88"/>
-      <c r="E32" s="82"/>
-      <c r="G32" s="86" t="s">
+      <c r="C32" s="86">
+        <v>0</v>
+      </c>
+      <c r="D32" s="87"/>
+      <c r="E32" s="34"/>
+      <c r="G32" s="38" t="s">
         <v>27</v>
       </c>
       <c r="H32" s="80">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I32" s="81"/>
-      <c r="K32" s="12"/>
+      <c r="K32" s="102"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="89" t="s">
+    <row r="33" spans="1:11" ht="15.75" customHeight="1">
+      <c r="B33" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="90"/>
-      <c r="D33" s="91">
+      <c r="C33" s="89"/>
+      <c r="D33" s="39">
         <f>SUM(C29:D32)</f>
-        <v>0.1041666667</v>
-      </c>
-      <c r="E33" s="66"/>
-      <c r="G33" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="28"/>
+      <c r="G33" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="H33" s="90"/>
-      <c r="I33" s="93">
+      <c r="H33" s="89"/>
+      <c r="I33" s="40">
         <f>SUM(H29:I32)</f>
         <v>0</v>
       </c>
-      <c r="K33" s="12"/>
+      <c r="K33" s="102"/>
     </row>
-    <row r="34" ht="9.75" customHeight="1">
-      <c r="B34" s="97"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="66"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="66"/>
-      <c r="K34" s="12"/>
+    <row r="34" spans="1:11" ht="9.75" customHeight="1">
+      <c r="B34" s="43"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="28"/>
+      <c r="K34" s="102"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="98"/>
-      <c r="B35" s="99" t="s">
+    <row r="35" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A35" s="44"/>
+      <c r="B35" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="100">
+      <c r="C35" s="91">
         <f>SUM(D24,D33)</f>
-        <v>0.1041666667</v>
-      </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="101"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="102" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="74"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H35" s="103">
+      <c r="H35" s="92">
         <f>SUM(I24,I33)</f>
-        <v>1.3125</v>
-      </c>
-      <c r="I35" s="104"/>
-      <c r="J35" s="105"/>
-      <c r="K35" s="12"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="93"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="102"/>
     </row>
-    <row r="36" ht="1.5" customHeight="1">
-      <c r="B36" s="106"/>
-      <c r="H36" s="106"/>
-      <c r="I36" s="106"/>
-      <c r="K36" s="12"/>
+    <row r="36" spans="1:11" ht="1.5" customHeight="1">
+      <c r="B36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="K36" s="102"/>
     </row>
-    <row r="37" ht="28.5" customHeight="1">
-      <c r="B37" s="107" t="s">
+    <row r="37" spans="1:11" ht="28.5" customHeight="1">
+      <c r="B37" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="108">
+      <c r="C37" s="70"/>
+      <c r="D37" s="50">
         <f>SUM((G9-C35)-(D33+D24))/G9*100</f>
-        <v>99.97106481</v>
-      </c>
-      <c r="E37" s="109"/>
-      <c r="G37" s="107" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="51"/>
+      <c r="G37" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="H37" s="20"/>
-      <c r="I37" s="110">
+      <c r="H37" s="70"/>
+      <c r="I37" s="52">
         <f>((G9-H35)-(I33+I24))/G9*100</f>
-        <v>99.63541667</v>
-      </c>
-      <c r="K37" s="111"/>
+        <v>100</v>
+      </c>
+      <c r="K37" s="103"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -3493,11 +3876,39 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="F11:H12"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="B2:I3"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="H29:I29"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="G16:I16"/>
@@ -3508,46 +3919,17 @@
     <mergeCell ref="Q18:Q19"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="B2:I3"/>
     <mergeCell ref="K5:K37"/>
     <mergeCell ref="N5:S7"/>
-    <mergeCell ref="H9:I9"/>
     <mergeCell ref="N9:Q9"/>
     <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="F11:H12"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactors GenerateMonitorReport and improves Excel formatting
The signature of GenerateMonitorReport in IReportService and ReportService has been changed to use DateTime instead of string for the dateFrom and dateTo parameters. In GenerateMonitorReportCommandHandler, the call to pass DateTime objects has been adjusted. In ReportService, the date range in Excel is now displayed in dd/MM/yyyy format. The calculation and writing of the total time difference between dateFrom and dateTo in cell (9,7) has been added. DownTime is now displayed in hh:mm:ss format instead of hh:mm.
</commit_message>
<xml_diff>
--- a/Uptime.Stars.Backend/Uptime.Stars.Api/Resources/ReportTemplate.xlsx
+++ b/Uptime.Stars.Backend/Uptime.Stars.Api/Resources/ReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseb\source\repos\Hackaton\uptime-stars-backend\Uptime.Stars.Backend\Uptime.Stars.Api\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19959433-410F-4525-BE96-6B7015B204CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AAF523-4722-4270-A9EA-7F8A8343B06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
-    <t>FEBRERO</t>
-  </si>
-  <si>
     <t xml:space="preserve">Service Availability (%) = </t>
   </si>
   <si>
@@ -60,25 +57,6 @@
   </si>
   <si>
     <t>Total period</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t>Data de 1 mes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t xml:space="preserve"> (horas)</t>
-    </r>
   </si>
   <si>
     <t>Caída de sistema por motivos internos - PD</t>
@@ -151,6 +129,28 @@
   </si>
   <si>
     <t>SLA EXTERNO = VENDORS %</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">Data de periodo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>(horas)</t>
+    </r>
+  </si>
+  <si>
+    <t>PERIODO</t>
   </si>
 </sst>
 </file>
@@ -1219,18 +1219,110 @@
     <xf numFmtId="2" fontId="9" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="46" fontId="7" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="7" fillId="7" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="6" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="6" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="7" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1239,98 +1331,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="7" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="46" fontId="6" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="6" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="7" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="7" fillId="7" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,7 +1395,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:srgbClr val="44C1A3"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1684,7 +1684,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="99CB38"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -2251,8 +2251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:S1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:D29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -2277,16 +2277,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="15" customHeight="1">
-      <c r="B2" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="97"/>
+      <c r="B2" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="1"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -2299,14 +2299,14 @@
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="2:19" ht="15" customHeight="1">
-      <c r="B3" s="98"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="100"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
       <c r="J3" s="1"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -2321,7 +2321,7 @@
     <row r="4" spans="2:19" ht="7.5" customHeight="1"/>
     <row r="5" spans="2:19" ht="18">
       <c r="B5" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -2330,19 +2330,19 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="K5" s="101"/>
-      <c r="N5" s="104" t="s">
-        <v>2</v>
-      </c>
-      <c r="O5" s="96"/>
-      <c r="P5" s="96"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="97"/>
+      <c r="K5" s="97"/>
+      <c r="N5" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="61"/>
     </row>
     <row r="6" spans="2:19" ht="18">
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2351,17 +2351,17 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="K6" s="102"/>
-      <c r="N6" s="105"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="107"/>
+      <c r="K6" s="98"/>
+      <c r="N6" s="101"/>
+      <c r="O6" s="102"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="102"/>
+      <c r="R6" s="102"/>
+      <c r="S6" s="103"/>
     </row>
     <row r="7" spans="2:19" ht="18">
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2370,123 +2370,123 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="K7" s="102"/>
-      <c r="N7" s="98"/>
-      <c r="O7" s="99"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="99"/>
-      <c r="R7" s="99"/>
-      <c r="S7" s="100"/>
+      <c r="K7" s="98"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="64"/>
     </row>
     <row r="8" spans="2:19" ht="14.4">
-      <c r="K8" s="102"/>
+      <c r="K8" s="98"/>
     </row>
     <row r="9" spans="2:19" ht="14.4">
       <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="F9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="7">
+        <v>24</v>
+      </c>
+      <c r="H9" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="58"/>
+      <c r="K9" s="98"/>
+      <c r="N9" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="7">
-        <v>720</v>
-      </c>
-      <c r="H9" s="108" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="70"/>
-      <c r="K9" s="102"/>
-      <c r="N9" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="74"/>
+      <c r="O9" s="88"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="54"/>
     </row>
     <row r="10" spans="2:19" ht="14.4">
       <c r="B10" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="9">
         <f>SUM(D33,I33)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="102"/>
+      <c r="K10" s="98"/>
       <c r="N10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="P10" s="11" t="s">
-        <v>13</v>
-      </c>
       <c r="Q10" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:19" ht="14.4">
       <c r="B11" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="14">
         <f>SUM(D24,I24)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="82"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="60"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="53">
+      <c r="D11" s="77"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="107" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="108"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="105">
         <f>((G9-C12)-(C10+C11))/G9*100</f>
         <v>100</v>
       </c>
-      <c r="K11" s="102"/>
-      <c r="N11" s="55">
+      <c r="K11" s="98"/>
+      <c r="N11" s="91">
         <f>((G9-N13)-(C29+C20))/G9*100</f>
         <v>100</v>
       </c>
-      <c r="O11" s="57">
+      <c r="O11" s="89">
         <f>((G9-O13)-(C30+C21))/G9*100</f>
         <v>100</v>
       </c>
-      <c r="P11" s="55">
+      <c r="P11" s="91">
         <f>((G9-P13)-(C31+C22))/G9*100</f>
         <v>100</v>
       </c>
-      <c r="Q11" s="55">
+      <c r="Q11" s="91">
         <f>((G9-Q13)-(C32+C23))/G9*100</f>
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="2:19" ht="14.4">
       <c r="B12" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" s="16">
         <f>SUM(C10:C11)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="84"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="54"/>
-      <c r="K12" s="102"/>
-      <c r="N12" s="56"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="56"/>
-      <c r="Q12" s="109"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="110"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="106"/>
+      <c r="K12" s="98"/>
+      <c r="N12" s="92"/>
+      <c r="O12" s="90"/>
+      <c r="P12" s="92"/>
+      <c r="Q12" s="104"/>
     </row>
     <row r="13" spans="2:19" ht="14.4">
-      <c r="K13" s="102"/>
+      <c r="K13" s="98"/>
       <c r="N13" s="17">
         <f>SUM(C20,C29)</f>
         <v>0</v>
@@ -2505,132 +2505,132 @@
       </c>
     </row>
     <row r="14" spans="2:19" ht="4.5" customHeight="1">
-      <c r="B14" s="65"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="67"/>
-      <c r="K14" s="102"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="84"/>
+      <c r="K14" s="98"/>
       <c r="N14" s="21"/>
       <c r="O14" s="22"/>
       <c r="P14" s="22"/>
       <c r="Q14" s="23"/>
     </row>
     <row r="15" spans="2:19" ht="14.4">
-      <c r="K15" s="102"/>
+      <c r="K15" s="98"/>
       <c r="N15" s="24"/>
       <c r="O15" s="25"/>
       <c r="P15" s="25"/>
       <c r="Q15" s="26"/>
     </row>
     <row r="16" spans="2:19" ht="14.4">
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="85" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="76"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="27"/>
+      <c r="G16" s="86" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="76"/>
+      <c r="I16" s="58"/>
+      <c r="K16" s="98"/>
+      <c r="N16" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="27"/>
-      <c r="G16" s="71" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="69"/>
-      <c r="I16" s="70"/>
-      <c r="K16" s="102"/>
-      <c r="N16" s="72" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="74"/>
+      <c r="O16" s="88"/>
+      <c r="P16" s="88"/>
+      <c r="Q16" s="54"/>
     </row>
     <row r="17" spans="2:17" ht="14.4">
       <c r="B17" s="28"/>
-      <c r="K17" s="102"/>
+      <c r="K17" s="98"/>
       <c r="N17" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O17" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="P17" s="11" t="s">
-        <v>13</v>
-      </c>
       <c r="Q17" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="2:17" ht="14.4">
-      <c r="B18" s="85" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="69"/>
-      <c r="D18" s="70"/>
+      <c r="B18" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="76"/>
+      <c r="D18" s="58"/>
       <c r="E18" s="30"/>
-      <c r="G18" s="77" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="69"/>
-      <c r="I18" s="70"/>
-      <c r="K18" s="102"/>
-      <c r="N18" s="57">
+      <c r="G18" s="80" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="76"/>
+      <c r="I18" s="58"/>
+      <c r="K18" s="98"/>
+      <c r="N18" s="89">
         <f>((G9-N20)-(H29+H20))/G9*100</f>
         <v>100</v>
       </c>
-      <c r="O18" s="55">
+      <c r="O18" s="91">
         <f>((G9-O20)-(H30+H21))/G9*100</f>
         <v>100</v>
       </c>
-      <c r="P18" s="55">
+      <c r="P18" s="91">
         <f>((G9-P20)-(H31+H22))/G9*100</f>
         <v>100</v>
       </c>
-      <c r="Q18" s="75">
+      <c r="Q18" s="93">
         <f>((G9-Q20)-(H32+H23))/G9*100</f>
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:17" ht="14.4">
       <c r="B19" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="110" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="111"/>
+        <v>19</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="67"/>
       <c r="E19" s="27"/>
       <c r="G19" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="78" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="79"/>
-      <c r="K19" s="102"/>
-      <c r="N19" s="58"/>
-      <c r="O19" s="56"/>
-      <c r="P19" s="56"/>
-      <c r="Q19" s="76"/>
+        <v>19</v>
+      </c>
+      <c r="H19" s="95" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="96"/>
+      <c r="K19" s="98"/>
+      <c r="N19" s="90"/>
+      <c r="O19" s="92"/>
+      <c r="P19" s="92"/>
+      <c r="Q19" s="94"/>
     </row>
     <row r="20" spans="2:17" ht="14.4">
       <c r="B20" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="80">
+        <v>21</v>
+      </c>
+      <c r="C20" s="68">
         <v>0</v>
       </c>
-      <c r="D20" s="81"/>
+      <c r="D20" s="69"/>
       <c r="E20" s="34"/>
       <c r="G20" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="80">
+        <v>21</v>
+      </c>
+      <c r="H20" s="68">
         <v>0</v>
       </c>
-      <c r="I20" s="81"/>
-      <c r="K20" s="102"/>
+      <c r="I20" s="69"/>
+      <c r="K20" s="98"/>
       <c r="N20" s="36">
         <f>SUM(H20,H29)</f>
         <v>0</v>
@@ -2650,207 +2650,207 @@
     </row>
     <row r="21" spans="2:17" ht="15.75" customHeight="1">
       <c r="B21" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="80">
+        <v>22</v>
+      </c>
+      <c r="C21" s="68">
         <v>0</v>
       </c>
-      <c r="D21" s="81"/>
+      <c r="D21" s="69"/>
       <c r="E21" s="34"/>
       <c r="G21" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" s="80">
+        <v>22</v>
+      </c>
+      <c r="H21" s="68">
         <v>0</v>
       </c>
-      <c r="I21" s="81"/>
-      <c r="K21" s="102"/>
+      <c r="I21" s="69"/>
+      <c r="K21" s="98"/>
     </row>
     <row r="22" spans="2:17" ht="15.75" customHeight="1">
       <c r="B22" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="80">
+        <v>23</v>
+      </c>
+      <c r="C22" s="68">
         <v>0</v>
       </c>
-      <c r="D22" s="81"/>
+      <c r="D22" s="69"/>
       <c r="E22" s="34"/>
       <c r="G22" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="80">
+        <v>24</v>
+      </c>
+      <c r="H22" s="68">
         <v>0</v>
       </c>
-      <c r="I22" s="81"/>
-      <c r="K22" s="102"/>
+      <c r="I22" s="69"/>
+      <c r="K22" s="98"/>
     </row>
     <row r="23" spans="2:17" ht="15.75" customHeight="1">
       <c r="B23" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="80">
+        <v>25</v>
+      </c>
+      <c r="C23" s="68">
         <v>0</v>
       </c>
-      <c r="D23" s="81"/>
+      <c r="D23" s="69"/>
       <c r="E23" s="34"/>
       <c r="G23" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" s="86">
+        <v>25</v>
+      </c>
+      <c r="H23" s="70">
         <v>0</v>
       </c>
-      <c r="I23" s="87"/>
-      <c r="K23" s="102"/>
+      <c r="I23" s="71"/>
+      <c r="K23" s="98"/>
     </row>
     <row r="24" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B24" s="88" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="89"/>
+      <c r="B24" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="73"/>
       <c r="D24" s="39">
         <f>SUM(C20:D23)</f>
         <v>0</v>
       </c>
       <c r="E24" s="28"/>
-      <c r="G24" s="90" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24" s="89"/>
+      <c r="G24" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="73"/>
       <c r="I24" s="40">
         <f>SUM(H20:I23)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="102"/>
+      <c r="K24" s="98"/>
     </row>
     <row r="25" spans="2:17" ht="15.75" customHeight="1">
-      <c r="K25" s="102"/>
+      <c r="K25" s="98"/>
     </row>
     <row r="26" spans="2:17" ht="15.75" customHeight="1">
-      <c r="K26" s="102"/>
+      <c r="K26" s="98"/>
     </row>
     <row r="27" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B27" s="85" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="69"/>
-      <c r="D27" s="70"/>
+      <c r="B27" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="76"/>
+      <c r="D27" s="58"/>
       <c r="E27" s="30"/>
-      <c r="G27" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="69"/>
-      <c r="I27" s="70"/>
-      <c r="K27" s="102"/>
+      <c r="G27" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="76"/>
+      <c r="I27" s="58"/>
+      <c r="K27" s="98"/>
     </row>
     <row r="28" spans="2:17" ht="15.75" customHeight="1">
       <c r="B28" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="110" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="111"/>
+        <v>19</v>
+      </c>
+      <c r="C28" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="67"/>
       <c r="E28" s="27"/>
       <c r="G28" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="H28" s="112" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="111"/>
-      <c r="K28" s="102"/>
+        <v>19</v>
+      </c>
+      <c r="H28" s="81" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="67"/>
+      <c r="K28" s="98"/>
     </row>
     <row r="29" spans="2:17" ht="15.75" customHeight="1">
       <c r="B29" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="80">
+        <v>21</v>
+      </c>
+      <c r="C29" s="68">
         <v>0</v>
       </c>
-      <c r="D29" s="81"/>
+      <c r="D29" s="69"/>
       <c r="E29" s="34"/>
       <c r="G29" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="80">
+        <v>21</v>
+      </c>
+      <c r="H29" s="68">
         <v>0</v>
       </c>
-      <c r="I29" s="81"/>
-      <c r="K29" s="102"/>
+      <c r="I29" s="69"/>
+      <c r="K29" s="98"/>
     </row>
     <row r="30" spans="2:17" ht="15.75" customHeight="1">
       <c r="B30" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="80">
+        <v>22</v>
+      </c>
+      <c r="C30" s="68">
         <v>0</v>
       </c>
-      <c r="D30" s="81"/>
+      <c r="D30" s="69"/>
       <c r="E30" s="34"/>
       <c r="G30" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="H30" s="80">
+        <v>22</v>
+      </c>
+      <c r="H30" s="68">
         <v>0</v>
       </c>
-      <c r="I30" s="81"/>
-      <c r="K30" s="102"/>
+      <c r="I30" s="69"/>
+      <c r="K30" s="98"/>
     </row>
     <row r="31" spans="2:17" ht="15.75" customHeight="1">
       <c r="B31" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="80">
+        <v>23</v>
+      </c>
+      <c r="C31" s="68">
         <v>0</v>
       </c>
-      <c r="D31" s="81"/>
+      <c r="D31" s="69"/>
       <c r="E31" s="34"/>
       <c r="G31" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="80">
+        <v>23</v>
+      </c>
+      <c r="H31" s="68">
         <v>0</v>
       </c>
-      <c r="I31" s="81"/>
-      <c r="K31" s="102"/>
+      <c r="I31" s="69"/>
+      <c r="K31" s="98"/>
     </row>
     <row r="32" spans="2:17" ht="15.75" customHeight="1">
       <c r="B32" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="86">
+        <v>25</v>
+      </c>
+      <c r="C32" s="70">
         <v>0</v>
       </c>
-      <c r="D32" s="87"/>
+      <c r="D32" s="71"/>
       <c r="E32" s="34"/>
       <c r="G32" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" s="80">
+        <v>25</v>
+      </c>
+      <c r="H32" s="68">
         <v>0</v>
       </c>
-      <c r="I32" s="81"/>
-      <c r="K32" s="102"/>
+      <c r="I32" s="69"/>
+      <c r="K32" s="98"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1">
-      <c r="B33" s="88" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="89"/>
+      <c r="B33" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="73"/>
       <c r="D33" s="39">
         <f>SUM(C29:D32)</f>
         <v>0</v>
       </c>
       <c r="E33" s="28"/>
-      <c r="G33" s="90" t="s">
-        <v>28</v>
-      </c>
-      <c r="H33" s="89"/>
+      <c r="G33" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="73"/>
       <c r="I33" s="40">
         <f>SUM(H29:I32)</f>
         <v>0</v>
       </c>
-      <c r="K33" s="102"/>
+      <c r="K33" s="98"/>
     </row>
     <row r="34" spans="1:11" ht="9.75" customHeight="1">
       <c r="B34" s="43"/>
@@ -2860,56 +2860,56 @@
       <c r="G34" s="27"/>
       <c r="H34" s="27"/>
       <c r="I34" s="28"/>
-      <c r="K34" s="102"/>
+      <c r="K34" s="98"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
       <c r="A35" s="44"/>
       <c r="B35" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="91">
+        <v>27</v>
+      </c>
+      <c r="C35" s="53">
         <f>SUM(D24,D33)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="74"/>
+      <c r="D35" s="54"/>
       <c r="E35" s="46"/>
       <c r="F35" s="22"/>
       <c r="G35" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="H35" s="92">
+        <v>28</v>
+      </c>
+      <c r="H35" s="55">
         <f>SUM(I24,I33)</f>
         <v>0</v>
       </c>
-      <c r="I35" s="93"/>
+      <c r="I35" s="56"/>
       <c r="J35" s="48"/>
-      <c r="K35" s="102"/>
+      <c r="K35" s="98"/>
     </row>
     <row r="36" spans="1:11" ht="1.5" customHeight="1">
       <c r="B36" s="49"/>
       <c r="H36" s="49"/>
       <c r="I36" s="49"/>
-      <c r="K36" s="102"/>
+      <c r="K36" s="98"/>
     </row>
     <row r="37" spans="1:11" ht="28.5" customHeight="1">
-      <c r="B37" s="94" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="70"/>
+      <c r="B37" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="58"/>
       <c r="D37" s="50">
         <f>SUM((G9-C35)-(D33+D24))/G9*100</f>
         <v>100</v>
       </c>
       <c r="E37" s="51"/>
-      <c r="G37" s="94" t="s">
-        <v>32</v>
-      </c>
-      <c r="H37" s="70"/>
+      <c r="G37" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="58"/>
       <c r="I37" s="52">
         <f>((G9-H35)-(I33+I24))/G9*100</f>
         <v>100</v>
       </c>
-      <c r="K37" s="103"/>
+      <c r="K37" s="99"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="39" spans="1:11" ht="15.75" customHeight="1"/>
@@ -3876,6 +3876,42 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="F11:H12"/>
+    <mergeCell ref="K5:K37"/>
+    <mergeCell ref="N5:S7"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="G33:H33"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="H35:I35"/>
     <mergeCell ref="B37:C37"/>
@@ -3892,42 +3928,6 @@
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="B27:D27"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="K5:K37"/>
-    <mergeCell ref="N5:S7"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="F11:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>